<commit_message>
Updated excel with progress
</commit_message>
<xml_diff>
--- a/TFM_Control.xlsx
+++ b/TFM_Control.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreea/Desktop/TFM/git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreea/Desktop/TFM/git/qubart/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA170A4-97CD-CF4C-AE21-84C78BC13B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD42E871-7811-5F4B-9243-AB6AD1E140C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{4091B506-2A8F-0144-B053-BFAAD76CBB69}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{4091B506-2A8F-0144-B053-BFAAD76CBB69}"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>https://towardsdatascience.com/embedviz-simple-unsupervised-keyphrase-extraction-using-sentence-embeddings-97ed5e16ad00</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>Progress</t>
   </si>
   <si>
     <t>Problems/questions</t>
@@ -108,6 +105,21 @@
   </si>
   <si>
     <t>1, 4</t>
+  </si>
+  <si>
+    <t>Streamlit</t>
+  </si>
+  <si>
+    <t>Interface</t>
+  </si>
+  <si>
+    <t>https://streamlit.io/</t>
+  </si>
+  <si>
+    <t>Created streamlit interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created git project </t>
   </si>
 </sst>
 </file>
@@ -213,7 +225,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -254,9 +266,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -264,9 +288,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -558,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C936E4F-6AED-4248-AE39-37B2EC34C2E3}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -569,90 +590,98 @@
     <col min="1" max="1" width="10.7109375" style="3"/>
     <col min="2" max="2" width="17.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="36.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="41.85546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="46.85546875" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="10.7109375" style="1"/>
+    <col min="4" max="4" width="46.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="23" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="12">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="16">
         <v>44417</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="14" t="s">
+      <c r="C2" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="16"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="16"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>44418</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <f>A5+1</f>
         <v>44419</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="B6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="12">
+        <v>44423</v>
+      </c>
+      <c r="B7" s="13">
+        <v>5</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
     <mergeCell ref="B2:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -661,10 +690,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{208F3576-F207-8848-8004-81BB025C94C5}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -708,7 +737,7 @@
       <c r="A3" s="9">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -722,7 +751,7 @@
       <c r="A4" s="9">
         <v>3</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="9" t="s">
         <v>7</v>
       </c>
@@ -735,13 +764,27 @@
         <v>4</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>20</v>
+      <c r="D5" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="14">
+        <v>5</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added embeddings visualization, cleaned corpus
</commit_message>
<xml_diff>
--- a/TFM_Control.xlsx
+++ b/TFM_Control.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreea/Desktop/TFM/git/qubart/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD42E871-7811-5F4B-9243-AB6AD1E140C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275E026F-6B5B-9147-A263-581E630EA337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{4091B506-2A8F-0144-B053-BFAAD76CBB69}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>https://towardsdatascience.com/embedviz-simple-unsupervised-keyphrase-extraction-using-sentence-embeddings-97ed5e16ad00</t>
   </si>
@@ -120,6 +120,33 @@
   </si>
   <si>
     <t xml:space="preserve">Created git project </t>
+  </si>
+  <si>
+    <t>https://www.docker.com/blog/containerized-python-development-part-1/</t>
+  </si>
+  <si>
+    <t>Docker</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>https://towardsdatascience.com/visualizing-word-embedding-with-pca-and-t-sne-961a692509f5</t>
+  </si>
+  <si>
+    <t>Visualizing Word Embedding with PCA and t-SNE</t>
+  </si>
+  <si>
+    <t>Visualization</t>
+  </si>
+  <si>
+    <t>6, 7</t>
+  </si>
+  <si>
+    <t>Edited corpus:
+1. . -&gt; _
+2. Changed pronouns to the referred person
+3. Joined sentences that talked about same thing</t>
   </si>
 </sst>
 </file>
@@ -225,7 +252,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -245,6 +272,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -257,38 +296,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -579,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C936E4F-6AED-4248-AE39-37B2EC34C2E3}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -601,81 +634,103 @@
       <c r="B1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="16">
+      <c r="A2" s="15">
         <v>44417</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="21" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="16"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
+      <c r="A5" s="11">
         <v>44418</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="22" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
+      <c r="A6" s="11">
         <f>A5+1</f>
         <v>44419</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="22" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="12">
+      <c r="A7" s="11">
         <v>44423</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="12">
         <v>5</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="22" t="s">
         <v>16</v>
       </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="11">
+        <v>44426</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A9" s="11">
+        <v>44431</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -690,10 +745,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{208F3576-F207-8848-8004-81BB025C94C5}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -720,13 +775,13 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="9">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -734,13 +789,13 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="9">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -748,11 +803,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="9">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="9" t="s">
+      <c r="B4" s="18"/>
+      <c r="C4" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -760,31 +815,59 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="11">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="14">
+      <c r="A6" s="9">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="9" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="13">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="13">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ROUGE metric, user input summary
</commit_message>
<xml_diff>
--- a/TFM_Control.xlsx
+++ b/TFM_Control.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreea/Desktop/TFM/git/qubart/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275E026F-6B5B-9147-A263-581E630EA337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06ACA058-1CEC-D24B-AB4B-819CB17BCE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{4091B506-2A8F-0144-B053-BFAAD76CBB69}"/>
   </bookViews>
@@ -146,7 +146,8 @@
     <t>Edited corpus:
 1. . -&gt; _
 2. Changed pronouns to the referred person
-3. Joined sentences that talked about same thing</t>
+3. Joined sentences that talked about same thing
+4. Deleted names of actors inside ()</t>
   </si>
 </sst>
 </file>
@@ -615,7 +616,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -720,7 +721,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>44431</v>
       </c>

</xml_diff>